<commit_message>
feature: Some changes in Front
</commit_message>
<xml_diff>
--- a/dev/ind comp2_OR_enviar.xlsx
+++ b/dev/ind comp2_OR_enviar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9707" tabRatio="918" firstSheet="9" activeTab="32"/>
+    <workbookView windowWidth="22176" windowHeight="9720" tabRatio="918" firstSheet="9" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="indicadores anuario" sheetId="1" r:id="rId1"/>
@@ -1808,7 +1808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2784" uniqueCount="1516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="1517">
   <si>
     <t>new_ID</t>
   </si>
@@ -6504,7 +6504,7 @@
     <t xml:space="preserve"> 3 774</t>
   </si>
   <si>
-    <t xml:space="preserve">  -   </t>
+    <t xml:space="preserve">  ...   </t>
   </si>
   <si>
     <t>2 024 046</t>
@@ -6688,6 +6688,9 @@
   </si>
   <si>
     <t>Porcentaje de campos de cultivo con presencia ilegal de OVM en el Perú, 2016-2023 (porcentaje)</t>
+  </si>
+  <si>
+    <t>...</t>
   </si>
   <si>
     <t>3,3</t>
@@ -7064,7 +7067,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="84">
+  <fonts count="83">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7405,13 +7408,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -7636,10 +7632,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -7649,11 +7646,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -7661,7 +7657,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7851,12 +7847,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8291,26 +8281,29 @@
   </borders>
   <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="13" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -8319,126 +8312,123 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="57" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="58" fillId="15" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="15" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="15" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="15" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="16" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="16" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="63" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="64" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="65" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="67" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="67" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="67" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="66" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="70" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="69" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10227,13 +10217,15 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx2">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:prstDash val="solid"/>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -10363,6 +10355,7 @@
                 <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -10440,8 +10433,10 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -10488,6 +10483,7 @@
           <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:prstDash val="solid"/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -13415,13 +13411,15 @@
                 <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx2">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:prstDash val="solid"/>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -13556,6 +13554,7 @@
                 <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
+            <a:prstDash val="solid"/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -13611,8 +13610,10 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -13659,6 +13660,7 @@
           <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:prstDash val="solid"/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -15222,10 +15224,13 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -15339,86 +15344,6 @@
 </file>
 
 <file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -16282,1046 +16207,6 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk2">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700">
-        <a:solidFill>
-          <a:schemeClr val="lt2"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="282">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="15875">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="800" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="ltDnDiag">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="lt1"/>
-        </a:bgClr>
-      </a:pattFill>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17842,7 +16727,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18345,7 +17230,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18848,7 +17733,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -20358,27 +19243,33 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -20393,7 +19284,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -20401,7 +19292,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -20409,14 +19300,17 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -20425,8 +19319,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk2">
-        <a:lumMod val="75000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
@@ -20449,35 +19344,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="2"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="2"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="31750" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -20486,32 +19381,33 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="2"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt2"/>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -20527,16 +19423,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -20570,17 +19471,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -20589,14 +19490,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -20608,20 +19509,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -20635,16 +19542,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
+          <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -20653,17 +19561,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -20672,16 +19580,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -20690,24 +19599,27 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -20715,19 +19627,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -20735,17 +19639,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -20754,9 +19658,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -20765,14 +19672,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -20781,7 +19688,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -20790,7 +19700,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -20811,7 +19721,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -20820,8 +19733,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -21330,509 +20249,6 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="266">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22300,7 +20716,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22816,6 +21232,577 @@
       <a:ln>
         <a:noFill/>
       </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="282">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -23709,7 +22696,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>5080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -23723,8 +22710,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4648200" y="1125855"/>
-        <a:ext cx="5682615" cy="2251710"/>
+        <a:off x="4648200" y="1102360"/>
+        <a:ext cx="5682615" cy="2275205"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -32965,7 +31952,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{b05759da-cb4f-47b7-803f-c805c5984257}">
+          <x14:cfRule type="iconSet" priority="5" id="{078228ec-c51c-4c02-a1b9-ea4bf2e54efe}">
             <x14:iconSet iconSet="3Symbols" custom="1" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -32984,7 +31971,7 @@
           <xm:sqref>E21:N21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{4885e8bb-5ab2-4104-8857-e739b02227e1}">
+          <x14:cfRule type="iconSet" priority="4" id="{252f6adf-a94b-45a8-84cd-a22fb2573d81}">
             <x14:iconSet iconSet="3Symbols" custom="1" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -33003,7 +31990,7 @@
           <xm:sqref>E22:N22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{2930986f-5d01-4be1-9821-d4ee3a2d5970}">
+          <x14:cfRule type="iconSet" priority="1" id="{13bac380-5c29-464b-97c0-3a7a719e362b}">
             <x14:iconSet iconSet="3Symbols" custom="1" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -33022,7 +32009,7 @@
           <xm:sqref>E2:N18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{120611cc-6025-450b-92b1-6d446ef99a86}">
+          <x14:cfRule type="iconSet" priority="6" id="{56ba0b84-8396-4b1f-a5ae-3ffbee3abf91}">
             <x14:iconSet iconSet="3Symbols" custom="1" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -33041,7 +32028,7 @@
           <xm:sqref>E19:N20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{a10412d5-f933-445e-a8b6-bd3ff9015cc3}">
+          <x14:cfRule type="iconSet" priority="3" id="{ad443dea-a2ad-4779-94ad-91cd8670f647}">
             <x14:iconSet iconSet="3Symbols" custom="1" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -33060,7 +32047,7 @@
           <xm:sqref>E24:N27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{aaed6e3c-2143-4afb-93e2-d72d9abbe3eb}">
+          <x14:cfRule type="iconSet" priority="8" id="{589a2c9b-8cff-4310-994d-17f4d3375fe7}">
             <x14:iconSet iconSet="3Symbols" custom="1" showValue="0">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -33090,7 +32077,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -33289,7 +32276,9 @@
       <c r="C14" s="104" t="s">
         <v>672</v>
       </c>
-      <c r="D14" s="104"/>
+      <c r="D14" s="104">
+        <v>0</v>
+      </c>
       <c r="E14" s="104" t="s">
         <v>750</v>
       </c>
@@ -33320,7 +32309,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -33775,7 +32764,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -34032,7 +33021,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -34219,7 +33208,9 @@
       <c r="B13" s="104">
         <v>92</v>
       </c>
-      <c r="C13" s="104"/>
+      <c r="C13" s="104">
+        <v>0</v>
+      </c>
       <c r="D13" s="104" t="s">
         <v>820</v>
       </c>
@@ -34249,7 +33240,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
@@ -35837,8 +34828,8 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -35888,7 +34879,7 @@
       <c r="B4" s="44" t="s">
         <v>572</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" t="s">
         <v>110</v>
       </c>
     </row>
@@ -37212,7 +36203,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -37631,7 +36622,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -37887,7 +36878,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4"/>
@@ -38450,7 +37441,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -38705,8 +37696,8 @@
   <sheetPr/>
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4"/>
@@ -39211,7 +38202,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -39467,7 +38458,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4"/>
@@ -39510,18 +38501,30 @@
       <c r="A4" s="37" t="s">
         <v>538</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C4" s="38" t="s">
         <v>708</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="E4" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G4" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="28" t="s">
@@ -39534,15 +38537,23 @@
         <v>708</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="F5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="37" t="s">
@@ -39551,17 +38562,27 @@
       <c r="B6" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="C6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="G6" s="38" t="s">
         <v>708</v>
       </c>
       <c r="H6" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="I6" s="38"/>
+      <c r="I6" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="28" t="s">
@@ -39579,31 +38600,55 @@
       <c r="E7" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
+      <c r="F7" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="37" t="s">
         <v>545</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C8" s="38" t="s">
-        <v>1447</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+        <v>1448</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="28" t="s">
         <v>547</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C9" s="29" t="s">
         <v>708</v>
       </c>
@@ -39613,12 +38658,18 @@
       <c r="E9" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="F9" s="29"/>
+      <c r="F9" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="G9" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
+      <c r="H9" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="37" t="s">
@@ -39636,29 +38687,47 @@
       <c r="E10" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="F10" s="38"/>
+      <c r="F10" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="G10" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="H10" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="28" t="s">
         <v>549</v>
       </c>
-      <c r="B11" s="29"/>
+      <c r="B11" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C11" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="E11" s="29" t="s">
-        <v>1448</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+        <v>1449</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="37" t="s">
@@ -39671,15 +38740,23 @@
         <v>708</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>1449</v>
-      </c>
-      <c r="E12" s="38"/>
+        <v>1450</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="F12" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="G12" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="28" t="s">
@@ -39697,13 +38774,17 @@
       <c r="E13" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+      <c r="F13" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="H13" s="29" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -39713,104 +38794,168 @@
       <c r="B14" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="D14" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
+      <c r="E14" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="G14" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="H14" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="28" t="s">
         <v>553</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C15" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="E15" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
+      <c r="F15" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="37" t="s">
-        <v>1452</v>
-      </c>
-      <c r="B16" s="38"/>
+        <v>1453</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C16" s="38" t="s">
-        <v>1448</v>
-      </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+        <v>1449</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="28" t="s">
         <v>555</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+      <c r="B17" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="H17" s="29" t="s">
-        <v>1453</v>
-      </c>
-      <c r="I17" s="29"/>
+        <v>1454</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="37" t="s">
         <v>556</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="D18" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="E18" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="28" t="s">
         <v>557</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="C19" s="29" t="s">
         <v>708</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="I19" s="29" t="s">
         <v>708</v>
@@ -39820,120 +38965,184 @@
       <c r="A20" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C20" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="D20" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="28" t="s">
         <v>559</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C21" s="29" t="s">
         <v>708</v>
       </c>
       <c r="D21" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
+      <c r="E21" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="H21" s="29" t="s">
         <v>708</v>
       </c>
-      <c r="I21" s="29"/>
+      <c r="I21" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="37" t="s">
         <v>560</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
+      <c r="B22" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="H22" s="38" t="s">
-        <v>1460</v>
-      </c>
-      <c r="I22" s="38"/>
+        <v>1461</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="28" t="s">
         <v>561</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="B23" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="E23" s="29" t="s">
-        <v>1461</v>
-      </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
+        <v>1462</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H23" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="37" t="s">
         <v>562</v>
       </c>
-      <c r="B24" s="38"/>
+      <c r="B24" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C24" s="38" t="s">
         <v>708</v>
       </c>
       <c r="D24" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
+      <c r="E24" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="F25" s="40" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="I25" s="40" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="41" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="41" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="28" spans="1:1">
@@ -39953,7 +39162,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -39983,7 +39192,7 @@
         <v>568</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="3" ht="36" spans="1:3">
@@ -39994,7 +39203,7 @@
         <v>570</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -40016,7 +39225,7 @@
         <v>573</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="6" ht="48" spans="1:3">
@@ -40027,7 +39236,7 @@
         <v>575</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -40047,7 +39256,7 @@
         <v>579</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="9" ht="24" spans="1:3">
@@ -40058,7 +39267,7 @@
         <v>581</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -40091,7 +39300,7 @@
         <v>587</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -40102,7 +39311,7 @@
         <v>589</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="14" ht="24" spans="1:3">
@@ -40113,7 +39322,7 @@
         <v>591</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="15" ht="96" spans="1:3">
@@ -40124,7 +39333,7 @@
         <v>593</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -40135,7 +39344,7 @@
         <v>595</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -40146,7 +39355,7 @@
         <v>597</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -40155,7 +39364,7 @@
         <v>599</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -40164,7 +39373,7 @@
         <v>601</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -40186,7 +39395,7 @@
         <v>604</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
     </row>
   </sheetData>
@@ -40466,14 +39675,14 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="25" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -40536,29 +39745,55 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="28" t="s">
-        <v>1452</v>
-      </c>
-      <c r="B5" s="29"/>
+        <v>1453</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="C5" s="29">
         <v>1</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
+      <c r="D5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>1446</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
+      <c r="B6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>1446</v>
+      </c>
       <c r="H6" s="38">
         <v>4</v>
       </c>
@@ -40597,12 +39832,12 @@
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="41" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="41" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -40622,7 +39857,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -40652,7 +39887,7 @@
         <v>568</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="3" ht="48" spans="1:3">
@@ -40663,7 +39898,7 @@
         <v>570</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -40685,7 +39920,7 @@
         <v>573</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="6" ht="48" spans="1:3">
@@ -40696,7 +39931,7 @@
         <v>575</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>1492</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -40716,7 +39951,7 @@
         <v>579</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>1493</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="9" ht="24" spans="1:3">
@@ -40727,7 +39962,7 @@
         <v>581</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -40760,7 +39995,7 @@
         <v>587</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -40771,7 +40006,7 @@
         <v>589</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="14" ht="36" spans="1:3">
@@ -40782,7 +40017,7 @@
         <v>591</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="15" ht="96" spans="1:3">
@@ -40793,7 +40028,7 @@
         <v>593</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1496</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -40804,7 +40039,7 @@
         <v>595</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -40815,7 +40050,7 @@
         <v>597</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>1482</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -40824,7 +40059,7 @@
         <v>599</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>1483</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -40833,7 +40068,7 @@
         <v>601</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1484</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -40855,7 +40090,7 @@
         <v>604</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>1497</v>
+        <v>1498</v>
       </c>
     </row>
   </sheetData>
@@ -40879,14 +40114,14 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="25" t="s">
-        <v>1498</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -40930,24 +40165,24 @@
         <v>1223</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="F4" s="29" t="s">
         <v>1226</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
       <c r="H4" s="29" t="s">
         <v>1226</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>1499</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="30" t="s">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="B5" s="31"/>
     </row>
@@ -40969,7 +40204,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -41000,7 +40235,7 @@
         <v>568</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1501</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="3" ht="96" spans="1:3">
@@ -41011,7 +40246,7 @@
         <v>570</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -41022,7 +40257,7 @@
         <v>572</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="5" ht="96" spans="1:3">
@@ -41033,7 +40268,7 @@
         <v>573</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1504</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="6" ht="336" spans="1:3">
@@ -41044,7 +40279,7 @@
         <v>575</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="7" ht="24" spans="1:3">
@@ -41055,7 +40290,7 @@
         <v>577</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="8" ht="36" spans="1:3">
@@ -41064,7 +40299,7 @@
         <v>579</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>1507</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -41075,7 +40310,7 @@
         <v>581</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -41130,7 +40365,7 @@
         <v>591</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>1509</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="15" ht="60" spans="1:3">
@@ -41141,7 +40376,7 @@
         <v>593</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>1510</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -41152,7 +40387,7 @@
         <v>595</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>1511</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="17" ht="24" spans="1:3">
@@ -41163,7 +40398,7 @@
         <v>597</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>1512</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="18" ht="24" spans="1:3">
@@ -41172,7 +40407,7 @@
         <v>599</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>1513</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -41181,7 +40416,7 @@
         <v>601</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1514</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -41203,7 +40438,7 @@
         <v>604</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
     </row>
   </sheetData>
@@ -41667,7 +40902,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -41886,7 +41121,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -42143,7 +41378,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5555555555556" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -42387,7 +41622,7 @@
   <sheetPr/>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>